<commit_message>
recolor DNA damage figures
</commit_message>
<xml_diff>
--- a/figures/exploratory/dna_damage/tables/BU_OUD_Striatum_dnaDamVal.perSampleByCell.xlsx
+++ b/figures/exploratory/dna_damage/tables/BU_OUD_Striatum_dnaDamVal.perSampleByCell.xlsx
@@ -525,7 +525,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -562,6 +562,11 @@
           <t>p.value</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>celltype</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -570,19 +575,24 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.004952520152717578</v>
+        <v>0.005237570917737962</v>
       </c>
       <c r="C2">
-        <v>0.002278082407288931</v>
+        <v>0.001765807011484599</v>
       </c>
       <c r="D2">
-        <v>2.173986391744013</v>
+        <v>2.96610608275617</v>
       </c>
       <c r="E2">
-        <v>185.3742142966079</v>
+        <v>76.34068802134549</v>
       </c>
       <c r="F2">
-        <v>0.03097354337597628</v>
+        <v>0.004024241284508979</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Microglia</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -592,19 +602,24 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.004832820880521418</v>
+        <v>0.005117871645542164</v>
       </c>
       <c r="C3">
-        <v>0.002302045301568183</v>
+        <v>0.001798781290339208</v>
       </c>
       <c r="D3">
-        <v>2.099359590025982</v>
+        <v>2.845188391178482</v>
       </c>
       <c r="E3">
-        <v>185.4568268624636</v>
+        <v>80.13137236548458</v>
       </c>
       <c r="F3">
-        <v>0.03713842930128484</v>
+        <v>0.00563263916610259</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Endothelial</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -614,19 +629,24 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.003861923771656746</v>
+        <v>0.004146974536677158</v>
       </c>
       <c r="C4">
-        <v>0.002277797782391958</v>
+        <v>0.001765211947161378</v>
       </c>
       <c r="D4">
-        <v>1.695463838585912</v>
+        <v>2.349278534708464</v>
       </c>
       <c r="E4">
-        <v>185.3738483632451</v>
+        <v>76.2620154281329</v>
       </c>
       <c r="F4">
-        <v>0.09166638271391066</v>
+        <v>0.02139995384339828</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Oligos_Pre</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -636,19 +656,24 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.003794024929925714</v>
+        <v>0.004079075694946135</v>
       </c>
       <c r="C5">
-        <v>0.00227750461303979</v>
+        <v>0.001764168583079837</v>
       </c>
       <c r="D5">
-        <v>1.665869262438868</v>
+        <v>2.312180215694011</v>
       </c>
       <c r="E5">
-        <v>185.373471297024</v>
+        <v>76.1132943218489</v>
       </c>
       <c r="F5">
-        <v>0.09742840495485316</v>
+        <v>0.02347327185342079</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Interneurons</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -658,19 +683,24 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.002421997104862944</v>
+        <v>0.002707047869883303</v>
       </c>
       <c r="C6">
-        <v>0.002277828680677697</v>
+        <v>0.001765280720146236</v>
       </c>
       <c r="D6">
-        <v>1.063292040094233</v>
+        <v>1.533494270338517</v>
       </c>
       <c r="E6">
-        <v>185.3738880849196</v>
+        <v>76.27121195121346</v>
       </c>
       <c r="F6">
-        <v>0.2890326888383201</v>
+        <v>0.1292919146334109</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Astrocytes</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -680,19 +710,24 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.002307549129314009</v>
+        <v>0.002592599894334472</v>
       </c>
       <c r="C7">
-        <v>0.002277980462308499</v>
+        <v>0.001764141056642705</v>
       </c>
       <c r="D7">
-        <v>1.012980210978431</v>
+        <v>1.469610315213902</v>
       </c>
       <c r="E7">
-        <v>185.3740832357265</v>
+        <v>76.08395242125513</v>
       </c>
       <c r="F7">
-        <v>0.312389955320176</v>
+        <v>0.1457904234221268</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Oligos</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -702,63 +737,105 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.00166379588982139</v>
+        <v>0.001948846654841802</v>
       </c>
       <c r="C8">
-        <v>0.002277631410872862</v>
+        <v>0.00176403634475677</v>
       </c>
       <c r="D8">
-        <v>0.7304939165656171</v>
+        <v>1.104765590932603</v>
       </c>
       <c r="E8">
-        <v>185.3736343969977</v>
+        <v>76.08583330064657</v>
       </c>
       <c r="F8">
-        <v>0.4660105456204779</v>
+        <v>0.2727425945235774</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>D1-MSN</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>celltype4Mural:DSM.IV.OUDOUD</t>
+          <t>celltype4D2-MSN:DSM.IV.OUDOUD</t>
         </is>
       </c>
       <c r="B9">
-        <v>-0.0007339316115047544</v>
+        <v>0.0009584590446104238</v>
       </c>
       <c r="C9">
-        <v>0.002330943823450158</v>
+        <v>0.001764036668905779</v>
       </c>
       <c r="D9">
-        <v>-0.3148645643542031</v>
+        <v>0.5433328351416584</v>
       </c>
       <c r="E9">
-        <v>185.5832139719234</v>
+        <v>76.0822131047389</v>
       </c>
       <c r="F9">
-        <v>0.7532182179597662</v>
+        <v>0.5884890948944963</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>D2-MSN</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>celltype4D2-MSN:DSM.IV.OUDOUD</t>
+          <t>celltype4Mural:DSM.IV.OUDOUD</t>
         </is>
       </c>
       <c r="B10">
-        <v>0.0006734082795899748</v>
+        <v>-0.0004488808464833061</v>
       </c>
       <c r="C10">
-        <v>0.002277701259579948</v>
+        <v>0.001836770867981745</v>
       </c>
       <c r="D10">
-        <v>0.2956525912946829</v>
+        <v>-0.2443858699569528</v>
       </c>
       <c r="E10">
-        <v>185.3737242341451</v>
+        <v>84.10064528662075</v>
       </c>
       <c r="F10">
-        <v>0.7678263168579035</v>
+        <v>0.8075272301508385</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Mural</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>celltype4D1/D2-Hybrid:DSM.IV.OUDOUD</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>0.0002850507650206718</v>
+      </c>
+      <c r="C11">
+        <v>0.001764248264487787</v>
+      </c>
+      <c r="D11">
+        <v>0.1615706648312506</v>
+      </c>
+      <c r="E11">
+        <v>76.12620225943856</v>
+      </c>
+      <c r="F11">
+        <v>0.8720720085822798</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>D1/D2-Hybrid</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DNA dam values and stats
</commit_message>
<xml_diff>
--- a/figures/exploratory/dna_damage/tables/BU_OUD_Striatum_dnaDamVal.perSampleByCell.xlsx
+++ b/figures/exploratory/dna_damage/tables/BU_OUD_Striatum_dnaDamVal.perSampleByCell.xlsx
@@ -1,22 +1,135 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/badoiphan/Library/Caches/com.binarynights.ForkLift-3/FileCache/1D6F0903-D812-463A-BE96-D9EA7CBCE68D/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADCC102-9DE6-7A49-9216-C2205D804FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="6960" yWindow="1460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DNA_dam_score_by_sample" sheetId="1" r:id="rId1"/>
     <sheet name="DNA_dam_score_by_sampleCelltype" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+  <si>
+    <t>term</t>
+  </si>
+  <si>
+    <t>estimate</t>
+  </si>
+  <si>
+    <t>std.error</t>
+  </si>
+  <si>
+    <t>statistic</t>
+  </si>
+  <si>
+    <t>p.value</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
+  </si>
+  <si>
+    <t>DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>SexM</t>
+  </si>
+  <si>
+    <t>PMI</t>
+  </si>
+  <si>
+    <t>RIN</t>
+  </si>
+  <si>
+    <t>numCell</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>celltype</t>
+  </si>
+  <si>
+    <t>celltype4Microglia:DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>Microglia</t>
+  </si>
+  <si>
+    <t>celltype4Endothelial:DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>Endothelial</t>
+  </si>
+  <si>
+    <t>celltype4Oligos_Pre:DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>Oligos_Pre</t>
+  </si>
+  <si>
+    <t>celltype4Interneurons:DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>Interneurons</t>
+  </si>
+  <si>
+    <t>celltype4Astrocytes:DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>Astrocytes</t>
+  </si>
+  <si>
+    <t>celltype4Oligos:DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>Oligos</t>
+  </si>
+  <si>
+    <t>celltype4D1-MSN:DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>D1-MSN</t>
+  </si>
+  <si>
+    <t>celltype4D2-MSN:DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>D2-MSN</t>
+  </si>
+  <si>
+    <t>celltype4Mural:DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>Mural</t>
+  </si>
+  <si>
+    <t>celltype4D1/D2-Hybrid:DSM.IV.OUDOUD</t>
+  </si>
+  <si>
+    <t>D1/D2-Hybrid</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +177,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -110,7 +231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -142,9 +263,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,6 +315,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -351,171 +508,155 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>term</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>estimate</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>std.error</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>statistic</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>p.value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>(Intercept)</t>
-        </is>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>0.02718190563765608</v>
+        <v>2.718190563765608E-2</v>
       </c>
       <c r="C2">
-        <v>0.002182356610127954</v>
+        <v>2.1823566101279541E-3</v>
       </c>
       <c r="D2">
-        <v>12.45529970285762</v>
+        <v>12.455299702857619</v>
       </c>
       <c r="E2">
-        <v>5.915574729791016e-05</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DSM.IV.OUDOUD</t>
-        </is>
+        <v>5.9155747297910163E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>0.002055650011053044</v>
+        <v>2.0556500110530439E-3</v>
       </c>
       <c r="C3">
-        <v>0.0003633839669393184</v>
+        <v>3.6338396693931838E-4</v>
       </c>
       <c r="D3">
-        <v>5.656963977709884</v>
+        <v>5.6569639777098839</v>
       </c>
       <c r="E3">
-        <v>0.002398648474310375</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
+        <v>2.398648474310375E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>3.063526938633565e-05</v>
+        <v>3.0635269386335647E-5</v>
       </c>
       <c r="C4">
-        <v>3.22139371820171e-05</v>
+        <v>3.2213937182017102E-5</v>
       </c>
       <c r="D4">
-        <v>0.9509942610627949</v>
+        <v>0.95099426106279494</v>
       </c>
       <c r="E4">
-        <v>0.3852788639191602</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>SexM</t>
-        </is>
+        <v>0.38527886391916022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>0.0005056321739668319</v>
+        <v>5.0563217396683193E-4</v>
       </c>
       <c r="C5">
-        <v>0.0005071013882318208</v>
+        <v>5.0710138823182075E-4</v>
       </c>
       <c r="D5">
-        <v>0.9971027208777484</v>
+        <v>0.99710272087774843</v>
       </c>
       <c r="E5">
-        <v>0.3644922596632857</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>PMI</t>
-        </is>
+        <v>0.36449225966328569</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>-0.0003557899121871669</v>
+        <v>-3.5578991218716691E-4</v>
       </c>
       <c r="C6">
-        <v>6.394292727152849e-05</v>
+        <v>6.3942927271528488E-5</v>
       </c>
       <c r="D6">
-        <v>-5.564179298147138</v>
+        <v>-5.5641792981471383</v>
       </c>
       <c r="E6">
-        <v>0.002580112267678879</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>RIN</t>
-        </is>
+        <v>2.5801122676788789E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>0.0004479605167030686</v>
+        <v>4.4796051670306858E-4</v>
       </c>
       <c r="C7">
-        <v>0.0003053168439367727</v>
+        <v>3.0531684393677271E-4</v>
       </c>
       <c r="D7">
         <v>1.467198831636801</v>
       </c>
       <c r="E7">
-        <v>0.2022404158216967</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>numCell</t>
-        </is>
+        <v>0.20224041582169669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>5.61858947138501e-08</v>
+        <v>5.6185894713850103E-8</v>
       </c>
       <c r="C8">
-        <v>8.314361962366131e-08</v>
+        <v>8.3143619623661307E-8</v>
       </c>
       <c r="D8">
         <v>0.6757691686766607</v>
       </c>
       <c r="E8">
-        <v>0.5291744419908453</v>
+        <v>0.52917444199084529</v>
       </c>
     </row>
   </sheetData>
@@ -524,318 +665,272 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>term</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>estimate</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>std.error</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>statistic</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>df</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>p.value</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>celltype</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>celltype4Microglia:DSM.IV.OUDOUD</t>
-        </is>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>0.005237570917737962</v>
+        <v>5.2375709177379616E-3</v>
       </c>
       <c r="C2">
-        <v>0.001765807011484599</v>
+        <v>1.765807011484599E-3</v>
       </c>
       <c r="D2">
-        <v>2.96610608275617</v>
+        <v>2.9661060827561698</v>
       </c>
       <c r="E2">
-        <v>76.34068802134549</v>
+        <v>76.340688021345485</v>
       </c>
       <c r="F2">
-        <v>0.004024241284508979</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Microglia</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>celltype4Endothelial:DSM.IV.OUDOUD</t>
-        </is>
+        <v>4.0242412845089793E-3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
       </c>
       <c r="B3">
-        <v>0.005117871645542164</v>
+        <v>5.1178716455421644E-3</v>
       </c>
       <c r="C3">
-        <v>0.001798781290339208</v>
+        <v>1.7987812903392079E-3</v>
       </c>
       <c r="D3">
-        <v>2.845188391178482</v>
+        <v>2.8451883911784819</v>
       </c>
       <c r="E3">
         <v>80.13137236548458</v>
       </c>
       <c r="F3">
-        <v>0.00563263916610259</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Endothelial</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>celltype4Oligos_Pre:DSM.IV.OUDOUD</t>
-        </is>
+        <v>5.6326391661025901E-3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
       </c>
       <c r="B4">
-        <v>0.004146974536677158</v>
+        <v>4.1469745366771579E-3</v>
       </c>
       <c r="C4">
-        <v>0.001765211947161378</v>
+        <v>1.765211947161378E-3</v>
       </c>
       <c r="D4">
-        <v>2.349278534708464</v>
+        <v>2.3492785347084642</v>
       </c>
       <c r="E4">
-        <v>76.2620154281329</v>
+        <v>76.262015428132898</v>
       </c>
       <c r="F4">
-        <v>0.02139995384339828</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Oligos_Pre</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>celltype4Interneurons:DSM.IV.OUDOUD</t>
-        </is>
+        <v>2.1399953843398281E-2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>0.004079075694946135</v>
+        <v>4.0790756949461351E-3</v>
       </c>
       <c r="C5">
-        <v>0.001764168583079837</v>
+        <v>1.764168583079837E-3</v>
       </c>
       <c r="D5">
-        <v>2.312180215694011</v>
+        <v>2.3121802156940112</v>
       </c>
       <c r="E5">
-        <v>76.1132943218489</v>
+        <v>76.113294321848898</v>
       </c>
       <c r="F5">
-        <v>0.02347327185342079</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Interneurons</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>celltype4Astrocytes:DSM.IV.OUDOUD</t>
-        </is>
+        <v>2.3473271853420789E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
       </c>
       <c r="B6">
-        <v>0.002707047869883303</v>
+        <v>2.7070478698833032E-3</v>
       </c>
       <c r="C6">
-        <v>0.001765280720146236</v>
+        <v>1.765280720146236E-3</v>
       </c>
       <c r="D6">
         <v>1.533494270338517</v>
       </c>
       <c r="E6">
-        <v>76.27121195121346</v>
+        <v>76.271211951213459</v>
       </c>
       <c r="F6">
-        <v>0.1292919146334109</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Astrocytes</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>celltype4Oligos:DSM.IV.OUDOUD</t>
-        </is>
+        <v>0.12929191463341089</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
       </c>
       <c r="B7">
-        <v>0.002592599894334472</v>
+        <v>2.592599894334472E-3</v>
       </c>
       <c r="C7">
-        <v>0.001764141056642705</v>
+        <v>1.764141056642705E-3</v>
       </c>
       <c r="D7">
         <v>1.469610315213902</v>
       </c>
       <c r="E7">
-        <v>76.08395242125513</v>
+        <v>76.083952421255134</v>
       </c>
       <c r="F7">
-        <v>0.1457904234221268</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Oligos</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>celltype4D1-MSN:DSM.IV.OUDOUD</t>
-        </is>
+        <v>0.14579042342212681</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
       </c>
       <c r="B8">
-        <v>0.001948846654841802</v>
+        <v>1.948846654841802E-3</v>
       </c>
       <c r="C8">
-        <v>0.00176403634475677</v>
+        <v>1.7640363447567701E-3</v>
       </c>
       <c r="D8">
-        <v>1.104765590932603</v>
+        <v>1.1047655909326031</v>
       </c>
       <c r="E8">
         <v>76.08583330064657</v>
       </c>
       <c r="F8">
-        <v>0.2727425945235774</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>D1-MSN</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>celltype4D2-MSN:DSM.IV.OUDOUD</t>
-        </is>
+        <v>0.27274259452357741</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
       </c>
       <c r="B9">
-        <v>0.0009584590446104238</v>
+        <v>9.584590446104238E-4</v>
       </c>
       <c r="C9">
-        <v>0.001764036668905779</v>
+        <v>1.7640366689057789E-3</v>
       </c>
       <c r="D9">
-        <v>0.5433328351416584</v>
+        <v>0.54333283514165842</v>
       </c>
       <c r="E9">
-        <v>76.0822131047389</v>
+        <v>76.082213104738898</v>
       </c>
       <c r="F9">
         <v>0.5884890948944963</v>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>D2-MSN</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>celltype4Mural:DSM.IV.OUDOUD</t>
-        </is>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
       </c>
       <c r="B10">
-        <v>-0.0004488808464833061</v>
+        <v>-4.4888084648330611E-4</v>
       </c>
       <c r="C10">
-        <v>0.001836770867981745</v>
+        <v>1.836770867981745E-3</v>
       </c>
       <c r="D10">
         <v>-0.2443858699569528</v>
       </c>
       <c r="E10">
-        <v>84.10064528662075</v>
+        <v>84.100645286620747</v>
       </c>
       <c r="F10">
-        <v>0.8075272301508385</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Mural</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>celltype4D1/D2-Hybrid:DSM.IV.OUDOUD</t>
-        </is>
+        <v>0.80752723015083849</v>
+      </c>
+      <c r="G10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
       </c>
       <c r="B11">
-        <v>0.0002850507650206718</v>
+        <v>2.8505076502067177E-4</v>
       </c>
       <c r="C11">
-        <v>0.001764248264487787</v>
+        <v>1.7642482644877871E-3</v>
       </c>
       <c r="D11">
         <v>0.1615706648312506</v>
       </c>
       <c r="E11">
-        <v>76.12620225943856</v>
+        <v>76.126202259438557</v>
       </c>
       <c r="F11">
-        <v>0.8720720085822798</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>D1/D2-Hybrid</t>
-        </is>
+        <v>0.87207200858227985</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>